<commit_message>
retraining (student orgs 2)
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>tag</t>
   </si>
@@ -161,16 +161,31 @@
     <t>student_orgs</t>
   </si>
   <si>
-    <t>what are the student organizations in plm?</t>
-  </si>
-  <si>
-    <t>Basta alam mo na yon</t>
-  </si>
-  <si>
-    <t>what student organizations can i join in plm?</t>
-  </si>
-  <si>
-    <t>list all student organizations in plm</t>
+    <t>Can you list the student organizations that are available in PLM?</t>
+  </si>
+  <si>
+    <t>Basta alam mo na yon part 2</t>
+  </si>
+  <si>
+    <t>What kinds of student organizations can students join in PLM?</t>
+  </si>
+  <si>
+    <t>Are there any specific student organizations that are popular among PLM students?</t>
+  </si>
+  <si>
+    <t>Could you provide some information on the different student organizations that exist in PLM?</t>
+  </si>
+  <si>
+    <t>What are the student-led groups or clubs in PLM?</t>
+  </si>
+  <si>
+    <t>Can you tell me about the various student organizations that operate in PLM?</t>
+  </si>
+  <si>
+    <t>Which student organizations are currently active in PLM?</t>
+  </si>
+  <si>
+    <t>How many student organizations are there in PLM, and what are they?</t>
   </si>
   <si>
     <t>what_icto</t>
@@ -450,7 +465,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="49.5"/>
+    <col customWidth="1" min="2" max="2" width="71.75"/>
     <col customWidth="1" min="3" max="3" width="138.0"/>
   </cols>
   <sheetData>
@@ -685,6 +700,31 @@
     <row r="37">
       <c r="B37" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -720,13 +760,13 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retraining (student orgs 3)
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -161,31 +161,31 @@
     <t>student_orgs</t>
   </si>
   <si>
-    <t>Can you list the student organizations that are available in PLM?</t>
+    <t>Can you list the organizations that are available in PLM?</t>
   </si>
   <si>
     <t>Basta alam mo na yon part 2</t>
   </si>
   <si>
-    <t>What kinds of student organizations can students join in PLM?</t>
-  </si>
-  <si>
-    <t>Are there any specific student organizations that are popular among PLM students?</t>
-  </si>
-  <si>
-    <t>Could you provide some information on the different student organizations that exist in PLM?</t>
+    <t>What kinds of organizations can students join in PLM?</t>
+  </si>
+  <si>
+    <t>Are there any specific organizations that are popular among PLM students?</t>
+  </si>
+  <si>
+    <t>Could you provide some information on the different organizations that exist in PLM?</t>
   </si>
   <si>
     <t>What are the student-led groups or clubs in PLM?</t>
   </si>
   <si>
-    <t>Can you tell me about the various student organizations that operate in PLM?</t>
-  </si>
-  <si>
-    <t>Which student organizations are currently active in PLM?</t>
-  </si>
-  <si>
-    <t>How many student organizations are there in PLM, and what are they?</t>
+    <t>Can you tell me about the various organizations that operate in PLM?</t>
+  </si>
+  <si>
+    <t>Which organizations are currently active in PLM?</t>
+  </si>
+  <si>
+    <t>How many organizations are there in PLM, and what are they?</t>
   </si>
   <si>
     <t>what_icto</t>

</xml_diff>

<commit_message>
retraining (student orgs 6)
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>tag</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>How many organizations are there in PLM, and what are they?</t>
+  </si>
+  <si>
+    <t>what organizations can i join in plm?</t>
   </si>
   <si>
     <t>what_icto</t>
@@ -727,6 +730,11 @@
         <v>57</v>
       </c>
     </row>
+    <row r="43">
+      <c r="B43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -760,13 +768,13 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retraining (student orgs 7)
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>tag</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>what organizations can i join in plm?</t>
+  </si>
+  <si>
+    <t>list all organizations in plm</t>
+  </si>
+  <si>
+    <t>what various organizations can i join in plm?</t>
   </si>
   <si>
     <t>what_icto</t>
@@ -735,6 +741,16 @@
         <v>58</v>
       </c>
     </row>
+    <row r="44">
+      <c r="B44" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -768,13 +784,13 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying github action 2
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>tag</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Do you know ICTO?</t>
+  </si>
+  <si>
+    <t>Define ICTO</t>
   </si>
 </sst>
 </file>
@@ -817,6 +820,11 @@
         <v>66</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
change epochs to 400
</commit_message>
<xml_diff>
--- a/chatplm/data/chatplm_brain.xlsx
+++ b/chatplm/data/chatplm_brain.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="general" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="about_chatplm" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="general" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>tag</t>
   </si>
@@ -22,6 +23,51 @@
     <t>response</t>
   </si>
   <si>
+    <t>who_are_you</t>
+  </si>
+  <si>
+    <t>who are you?</t>
+  </si>
+  <si>
+    <t>Hi, haribon! I am ChatPLM, a simple AI trained to answer your PLM-related questions. Ask me anything about PLM and I'll try my best to answer it.</t>
+  </si>
+  <si>
+    <t>what is your name?</t>
+  </si>
+  <si>
+    <t>introduce yourself</t>
+  </si>
+  <si>
+    <t>tell me about yourself</t>
+  </si>
+  <si>
+    <t>tell me about you</t>
+  </si>
+  <si>
+    <t>who_created</t>
+  </si>
+  <si>
+    <t>who created you?</t>
+  </si>
+  <si>
+    <t>I am developed by a group of passionate Computer Science students from PLM and maintained by a lot of student volunteers!</t>
+  </si>
+  <si>
+    <t>who developed you?</t>
+  </si>
+  <si>
+    <t>who made you?</t>
+  </si>
+  <si>
+    <t>who are the people behind your development?</t>
+  </si>
+  <si>
+    <t>who are the people that created you?</t>
+  </si>
+  <si>
+    <t>who are the people that made you?</t>
+  </si>
+  <si>
     <t>courses_offered</t>
   </si>
   <si>
@@ -37,9 +83,6 @@
     <t>Can you tell me about PLM's academic programs?</t>
   </si>
   <si>
-    <t>What undergraduate and graduate courses are available at PLM?</t>
-  </si>
-  <si>
     <t>what are the courses in plm?</t>
   </si>
   <si>
@@ -70,6 +113,12 @@
     <t>Is PLM a public school?</t>
   </si>
   <si>
+    <t>is plm public?</t>
+  </si>
+  <si>
+    <t>is plm private?</t>
+  </si>
+  <si>
     <t>admission_process</t>
   </si>
   <si>
@@ -91,6 +140,9 @@
     <t>how to apply?</t>
   </si>
   <si>
+    <t>tell me about the admission process</t>
+  </si>
+  <si>
     <t>tuition_fee</t>
   </si>
   <si>
@@ -115,6 +167,9 @@
     <t>does plm have a tuition fee?</t>
   </si>
   <si>
+    <t>tell me about the tuition fee</t>
+  </si>
+  <si>
     <t>history</t>
   </si>
   <si>
@@ -136,28 +191,28 @@
     <t>tell me about plm's history</t>
   </si>
   <si>
-    <t>campus</t>
-  </si>
-  <si>
-    <t>What is the campus like at PLM?</t>
-  </si>
-  <si>
-    <t>PLM's main campus is located in the heart of Manila, near several major landmarks and attractions. The campus is well-maintained and features modern facilities, including lecture halls, laboratories, libraries, and sports facilities.</t>
+    <t>location</t>
   </si>
   <si>
     <t>Where is PLM located?</t>
   </si>
   <si>
-    <t>Can you describe the campus of PLM?</t>
-  </si>
-  <si>
-    <t>What facilities does PLM's campus have?</t>
+    <t>PLM's main campus is located in General Luna, corner Muralla St, Intramuros, Manila, 1002 Metro Manila.</t>
   </si>
   <si>
     <t>where can i find plm?</t>
   </si>
   <si>
     <t>i want to find where is plm. can you tell me?</t>
+  </si>
+  <si>
+    <t>tell me plm's location</t>
+  </si>
+  <si>
+    <t>give me plm's location</t>
+  </si>
+  <si>
+    <t>where is plm?</t>
   </si>
   <si>
     <t>student_orgs</t>
@@ -242,9 +297,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -261,6 +325,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -468,297 +536,432 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="25.38"/>
+    <col customWidth="1" min="3" max="3" width="48.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="1" max="1" width="18.88"/>
     <col customWidth="1" min="2" max="2" width="71.75"/>
     <col customWidth="1" min="3" max="3" width="138.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="s">
-        <v>8</v>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>9</v>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>10</v>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>15</v>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="s">
-        <v>16</v>
+      <c r="B11" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>17</v>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
-        <v>18</v>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="s">
-        <v>22</v>
+      <c r="A15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="s">
-        <v>23</v>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="s">
-        <v>24</v>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
+      <c r="B18" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
+      <c r="B19" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
-        <v>29</v>
+      <c r="B20" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="s">
-        <v>30</v>
+      <c r="A21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="2" t="s">
-        <v>31</v>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="2" t="s">
-        <v>32</v>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="2" t="s">
-        <v>33</v>
+      <c r="B24" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>36</v>
+      <c r="B25" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="2" t="s">
-        <v>37</v>
+      <c r="B26" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="2" t="s">
-        <v>38</v>
+      <c r="B27" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="2" t="s">
-        <v>39</v>
+      <c r="A28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="2" t="s">
-        <v>40</v>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>43</v>
+      <c r="B30" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="2" t="s">
-        <v>44</v>
+      <c r="B31" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="2" t="s">
-        <v>45</v>
+      <c r="B32" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="2" t="s">
-        <v>46</v>
+      <c r="A33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="2" t="s">
-        <v>47</v>
+      <c r="B34" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="2" t="s">
-        <v>48</v>
+      <c r="B35" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>51</v>
+      <c r="B36" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="2" t="s">
-        <v>52</v>
+      <c r="B37" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="2" t="s">
-        <v>53</v>
+      <c r="B38" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="2" t="s">
-        <v>54</v>
+      <c r="A39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="2" t="s">
-        <v>55</v>
+      <c r="B40" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="2" t="s">
-        <v>56</v>
+      <c r="B41" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="2" t="s">
-        <v>57</v>
+      <c r="B42" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="2" t="s">
-        <v>58</v>
+      <c r="B43" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="2" t="s">
-        <v>59</v>
+      <c r="B44" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="2" t="s">
-        <v>60</v>
+      <c r="B45" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="2" t="s">
-        <v>61</v>
+      <c r="B46" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="2" t="s">
-        <v>62</v>
+      <c r="B47" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="2" t="s">
-        <v>63</v>
+      <c r="B48" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>